<commit_message>
implémentation des caractéristiques des armes
</commit_message>
<xml_diff>
--- a/documentation/tableau équillibrage.xlsx
+++ b/documentation/tableau équillibrage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\iCloudDrive\cours\Semestre 2\UE 2.4 Projets\projet info\La-Bataille-Brestoise\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59404515-FAF0-4AB5-BBCA-EA2AE2746110}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BFA79C-67F1-4860-88D6-FE2C1171C778}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="1140" windowWidth="13500" windowHeight="17235" xr2:uid="{4D52B082-FC73-4ED9-BEC2-70DD9A2E8F34}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{4D52B082-FC73-4ED9-BEC2-70DD9A2E8F34}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>BE</t>
   </si>
@@ -102,9 +102,6 @@
     <t>DPS</t>
   </si>
   <si>
-    <t>degats instantannée</t>
-  </si>
-  <si>
     <t>calibre50</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
   </si>
   <si>
     <t>niveau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vitesse vol ( km/s) </t>
   </si>
   <si>
     <t xml:space="preserve">vitesse (km/s) </t>
@@ -753,15 +747,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CC2D8F-DB4D-4280-9201-88521C7DD6EB}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D67" sqref="D66:D67"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="19" t="s">
@@ -971,51 +965,51 @@
       <c r="B7" s="18"/>
       <c r="C7" s="28">
         <f>$B34/$B25+ D25</f>
-        <v>6</v>
+        <v>6.3529411764705888</v>
       </c>
       <c r="D7" s="28">
         <f>$B35/$B25+ D25</f>
-        <v>5.5</v>
+        <v>5.7647058823529411</v>
       </c>
       <c r="E7" s="28">
         <f>$B36/$B25+ D25</f>
-        <v>7</v>
+        <v>7.5294117647058822</v>
       </c>
       <c r="F7" s="28">
         <f>$B37/$B25+ D25</f>
-        <v>6</v>
+        <v>6.3529411764705888</v>
       </c>
       <c r="G7" s="28">
         <f>$B38/$B25+ D24+ D25</f>
-        <v>10</v>
+        <v>10.529411764705882</v>
       </c>
       <c r="H7" s="28">
         <f>$B39/$B25+ D25</f>
-        <v>8</v>
+        <v>8.7058823529411775</v>
       </c>
       <c r="I7" s="28">
         <f>$B40/$B25+ D25</f>
-        <v>10</v>
+        <v>11.058823529411764</v>
       </c>
       <c r="J7" s="28">
         <f>$B41/$B25+ D25</f>
-        <v>10</v>
+        <v>11.058823529411764</v>
       </c>
       <c r="K7" s="28">
         <f>$B42/$B25+ D25</f>
-        <v>12</v>
+        <v>13.411764705882353</v>
       </c>
       <c r="L7" s="28">
         <f>$B43/$B25+ D25</f>
-        <v>7</v>
+        <v>7.5294117647058822</v>
       </c>
       <c r="M7" s="28">
         <f>$B44/$B25+ D25</f>
-        <v>14</v>
+        <v>15.764705882352942</v>
       </c>
       <c r="N7" s="28">
         <f>$B45/$B25+ D25</f>
-        <v>10</v>
+        <v>11.058823529411764</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1041,51 +1035,51 @@
       <c r="B9" s="18"/>
       <c r="C9" s="28">
         <f>$B34/$B26+ D26</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="D9" s="28">
         <f>$B35/$B26+ D26</f>
-        <v>6.5</v>
+        <v>6.875</v>
       </c>
       <c r="E9" s="28">
         <f>$B36/$B26+ D26</f>
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="F9" s="28">
         <f>$B37/$B26+ D26</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="G9" s="28">
         <f>$B38/$B26+ D26</f>
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H9" s="28">
         <f>$B39/$B26+ D26</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I9" s="28">
         <f>$B40/$B26+ D26</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="J9" s="28">
         <f>$B41/$B26+ D26</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="K9" s="28">
         <f>$B42/$B26+ D26</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L9" s="28">
         <f>$B43/$B26+ D26</f>
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="M9" s="28">
         <f>$B44/$B26+ D26</f>
-        <v>15</v>
+        <v>17.5</v>
       </c>
       <c r="N9" s="28">
         <f>$B45/$B26+ D26</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1109,59 +1103,59 @@
         <v>16</v>
       </c>
       <c r="B11" s="18"/>
-      <c r="C11" s="29">
-        <f>((B34/C27)+1)*D27</f>
-        <v>11.666666666666664</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="C11" s="28">
+        <f t="shared" ref="C11" si="0">$B36/$B28+ D28</f>
+        <v>11</v>
+      </c>
+      <c r="D11" s="29" t="e">
         <f>((B35/C27)+1)*D27</f>
-        <v>10</v>
-      </c>
-      <c r="E11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="29" t="e">
         <f>(($B36/$C$27)+1)*$D$27</f>
-        <v>15</v>
-      </c>
-      <c r="F11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="29" t="e">
         <f>(($B37/$C$27)+1)*$D$27</f>
-        <v>11.666666666666664</v>
-      </c>
-      <c r="G11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="29" t="e">
         <f>(($B38/$C$27)+1)*$D$27</f>
-        <v>15</v>
-      </c>
-      <c r="H11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="29" t="e">
         <f>(($B39/$C$27)+1)*$D$27</f>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="I11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="29" t="e">
         <f>(($B40/$C$27)+1)*$D$27</f>
-        <v>25</v>
-      </c>
-      <c r="J11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="29" t="e">
         <f>(($B41/$C$27)+1)*$D$27</f>
-        <v>25</v>
-      </c>
-      <c r="K11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="29" t="e">
         <f>(($B42/$C$27)+1)*$D$27</f>
-        <v>31.666666666666664</v>
-      </c>
-      <c r="L11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L11" s="29" t="e">
         <f>(($B43/$C$27)+1)*$D$27</f>
-        <v>15</v>
-      </c>
-      <c r="M11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="29" t="e">
         <f>(($B44/$C$27)+1)*$D$27</f>
-        <v>38.333333333333336</v>
-      </c>
-      <c r="N11" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="29" t="e">
         <f>(($B45/$C$27)+1)*$D$27</f>
-        <v>25</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="29"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -1179,59 +1173,59 @@
         <v>17</v>
       </c>
       <c r="B13" s="18"/>
-      <c r="C13" s="29">
-        <f>(($B34/$C$28)+1)*$D$28</f>
-        <v>16</v>
-      </c>
-      <c r="D13" s="29">
+      <c r="C13" s="28">
+        <f t="shared" ref="C13" si="1">$B38/$B30+ D30</f>
+        <v>12.5</v>
+      </c>
+      <c r="D13" s="29" t="e">
         <f>(($B35/$C$28)+1)*$D$28</f>
-        <v>14</v>
-      </c>
-      <c r="E13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="29" t="e">
         <f>(($B36/$C$28)+1)*$D$28</f>
-        <v>20</v>
-      </c>
-      <c r="F13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="29" t="e">
         <f>(($B37/$C$28)+1)*$D$28</f>
-        <v>16</v>
-      </c>
-      <c r="G13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="29" t="e">
         <f>(($B38/$C$28)+1)*$D$28</f>
-        <v>20</v>
-      </c>
-      <c r="H13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="29" t="e">
         <f>(($B39/$C$28)+1)*$D$28</f>
-        <v>24</v>
-      </c>
-      <c r="I13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="29" t="e">
         <f>(($B40/$C$28)+1)*$D$28</f>
-        <v>32</v>
-      </c>
-      <c r="J13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="29" t="e">
         <f>(($B41/$C$28)+1)*$D$28</f>
-        <v>32</v>
-      </c>
-      <c r="K13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="29" t="e">
         <f>(($B42/$C$28)+1)*$D$28</f>
-        <v>40</v>
-      </c>
-      <c r="L13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" s="29" t="e">
         <f>(($B43/$C$28)+1)*$D$28</f>
-        <v>20</v>
-      </c>
-      <c r="M13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="29" t="e">
         <f>(($B44/$C$28)+1)*$D$28</f>
-        <v>48</v>
-      </c>
-      <c r="N13" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="29" t="e">
         <f>(($B45/$C$28)+1)*$D$28</f>
-        <v>32</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="29"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -1249,59 +1243,59 @@
         <v>18</v>
       </c>
       <c r="B15" s="18"/>
-      <c r="C15" s="29">
-        <f>(($B34/$C$29)+1)*$D$29</f>
-        <v>17.692307692307693</v>
-      </c>
-      <c r="D15" s="29">
+      <c r="C15" s="28" t="e">
+        <f t="shared" ref="C15" si="2">$B40/$B32+ D32</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="29" t="e">
         <f>(($B35/$C$29)+1)*$D$29</f>
-        <v>15.769230769230768</v>
-      </c>
-      <c r="E15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="29" t="e">
         <f>(($B36/$C$29)+1)*$D$29</f>
-        <v>21.538461538461537</v>
-      </c>
-      <c r="F15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="29" t="e">
         <f>(($B37/$C$29)+1)*$D$29</f>
-        <v>17.692307692307693</v>
-      </c>
-      <c r="G15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="29" t="e">
         <f>(($B38/$C$29)+1)*$D$29</f>
-        <v>21.538461538461537</v>
-      </c>
-      <c r="H15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="29" t="e">
         <f>(($B39/$C$29)+1)*$D$29</f>
-        <v>25.384615384615383</v>
-      </c>
-      <c r="I15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="29" t="e">
         <f>(($B40/$C$29)+1)*$D$29</f>
-        <v>33.076923076923073</v>
-      </c>
-      <c r="J15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="29" t="e">
         <f>(($B41/$C$29)+1)*$D$29</f>
-        <v>33.076923076923073</v>
-      </c>
-      <c r="K15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="29" t="e">
         <f>(($B42/$C$29)+1)*$D$29</f>
-        <v>40.769230769230766</v>
-      </c>
-      <c r="L15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="29" t="e">
         <f>(($B43/$C$29)+1)*$D$29</f>
-        <v>21.538461538461537</v>
-      </c>
-      <c r="M15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="29" t="e">
         <f>(($B44/$C$29)+1)*$D$29</f>
-        <v>48.461538461538467</v>
-      </c>
-      <c r="N15" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="29" t="e">
         <f>(($B45/$C$29)+1)*$D$29</f>
-        <v>33.076923076923073</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="29"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
@@ -1319,59 +1313,59 @@
         <v>19</v>
       </c>
       <c r="B17" s="18"/>
-      <c r="C17" s="29">
-        <f>(($B34/$C$30)+1)*$D$30</f>
-        <v>20</v>
-      </c>
-      <c r="D17" s="29">
+      <c r="C17" s="28">
+        <f t="shared" ref="C17" si="3">$B42/$B34+ D34</f>
+        <v>5.75</v>
+      </c>
+      <c r="D17" s="29" t="e">
         <f>(($B35/$C$30)+1)*$D$30</f>
-        <v>18.75</v>
-      </c>
-      <c r="E17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="29" t="e">
         <f>(($B36/$C$30)+1)*$D$30</f>
-        <v>22.5</v>
-      </c>
-      <c r="F17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="29" t="e">
         <f>(($B37/$C$30)+1)*$D$30</f>
-        <v>20</v>
-      </c>
-      <c r="G17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="29" t="e">
         <f>(($B38/$C$30)+1)*$D$30</f>
-        <v>22.5</v>
-      </c>
-      <c r="H17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="29" t="e">
         <f>(($B39/$C$30)+1)*$D$30</f>
-        <v>24.999999999999996</v>
-      </c>
-      <c r="I17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="29" t="e">
         <f>(($B40/$C$30)+1)*$D$30</f>
-        <v>30</v>
-      </c>
-      <c r="J17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="29" t="e">
         <f>(($B41/$C$30)+1)*$D$30</f>
-        <v>30</v>
-      </c>
-      <c r="K17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="29" t="e">
         <f>(($B42/$C$30)+1)*$D$30</f>
-        <v>34.999999999999993</v>
-      </c>
-      <c r="L17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="29" t="e">
         <f>(($B43/$C$30)+1)*$D$30</f>
-        <v>22.5</v>
-      </c>
-      <c r="M17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="29" t="e">
         <f>(($B44/$C$30)+1)*$D$30</f>
-        <v>40.000000000000007</v>
-      </c>
-      <c r="N17" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" s="29" t="e">
         <f>(($B45/$C$30)+1)*$D$30</f>
-        <v>30</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="29"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
@@ -1389,59 +1383,59 @@
         <v>20</v>
       </c>
       <c r="B19" s="18"/>
-      <c r="C19" s="29">
-        <f>(($B34/$C$31)+1)*$D$31</f>
-        <v>19.285714285714285</v>
-      </c>
-      <c r="D19" s="29">
+      <c r="C19" s="28">
+        <f t="shared" ref="C19" si="4">$B44/$B36+ D36</f>
+        <v>6.3333333333333339</v>
+      </c>
+      <c r="D19" s="29" t="e">
         <f>(($B35/$C$31)+1)*$D$31</f>
-        <v>18.214285714285712</v>
-      </c>
-      <c r="E19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="29" t="e">
         <f>(($B36/$C$31)+1)*$D$31</f>
-        <v>21.428571428571431</v>
-      </c>
-      <c r="F19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="29" t="e">
         <f>(($B37/$C$31)+1)*$D$31</f>
-        <v>19.285714285714285</v>
-      </c>
-      <c r="G19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="29" t="e">
         <f>(($B38/$C$31)+1)*$D$31</f>
-        <v>21.428571428571431</v>
-      </c>
-      <c r="H19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="29" t="e">
         <f>(($B39/$C$31)+1)*$D$31</f>
-        <v>23.571428571428569</v>
-      </c>
-      <c r="I19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="29" t="e">
         <f>(($B40/$C$31)+1)*$D$31</f>
-        <v>27.857142857142858</v>
-      </c>
-      <c r="J19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="29" t="e">
         <f>(($B41/$C$31)+1)*$D$31</f>
-        <v>27.857142857142858</v>
-      </c>
-      <c r="K19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="29" t="e">
         <f>(($B42/$C$31)+1)*$D$31</f>
-        <v>32.142857142857139</v>
-      </c>
-      <c r="L19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="29" t="e">
         <f>(($B43/$C$31)+1)*$D$31</f>
-        <v>21.428571428571431</v>
-      </c>
-      <c r="M19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="29" t="e">
         <f>(($B44/$C$31)+1)*$D$31</f>
-        <v>36.428571428571431</v>
-      </c>
-      <c r="N19" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="29" t="e">
         <f>(($B45/$C$31)+1)*$D$31</f>
-        <v>27.857142857142858</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="29"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
@@ -1465,206 +1459,166 @@
       <c r="B22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>23</v>
-      </c>
+      <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>41</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5">
         <v>1000</v>
       </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
       </c>
-      <c r="F23" s="12">
-        <v>2</v>
-      </c>
+      <c r="F23" s="12"/>
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="5">
         <v>2000</v>
       </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="5">
         <v>3</v>
       </c>
       <c r="E24" s="5">
         <v>2</v>
       </c>
-      <c r="F24" s="7">
-        <v>2</v>
-      </c>
+      <c r="F24" s="7"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5">
-        <v>5000</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
+        <v>4250</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="5">
         <v>4</v>
       </c>
       <c r="E25" s="5">
         <v>6</v>
       </c>
-      <c r="F25" s="7">
-        <v>4</v>
-      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5">
-        <v>5000</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
+        <v>4000</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="5">
         <v>5</v>
       </c>
       <c r="E26" s="5">
         <v>8</v>
       </c>
-      <c r="F26" s="7">
-        <v>3.5</v>
-      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5">
-        <v>7500</v>
-      </c>
+        <v>4500</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="5">
         <v>5</v>
       </c>
       <c r="E27" s="5">
         <v>5</v>
       </c>
-      <c r="F27" s="7">
-        <v>2.5</v>
-      </c>
+      <c r="F27" s="7"/>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="5">
-        <v>0</v>
-      </c>
-      <c r="C28" s="5">
-        <v>10000</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="5">
         <v>8</v>
       </c>
       <c r="E28" s="5">
         <v>15</v>
       </c>
-      <c r="F28" s="7">
-        <v>4</v>
-      </c>
+      <c r="F28" s="7"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5">
-        <v>0</v>
-      </c>
-      <c r="C29" s="5">
-        <v>13000</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="C29" s="5"/>
       <c r="D29" s="5">
         <v>10</v>
       </c>
       <c r="E29" s="5">
         <v>20</v>
       </c>
-      <c r="F29" s="7">
-        <v>2</v>
-      </c>
+      <c r="F29" s="7"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5">
-        <v>30000</v>
-      </c>
+        <v>6000</v>
+      </c>
+      <c r="C30" s="5"/>
       <c r="D30" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E30" s="5">
         <v>30</v>
       </c>
-      <c r="F30" s="7">
-        <v>2</v>
-      </c>
+      <c r="F30" s="7"/>
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="9">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9">
-        <v>35000</v>
-      </c>
+        <v>6000</v>
+      </c>
+      <c r="C31" s="9"/>
       <c r="D31" s="9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E31" s="9">
         <v>30</v>
       </c>
-      <c r="F31" s="10">
-        <v>8</v>
-      </c>
+      <c r="F31" s="10"/>
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -1673,22 +1627,22 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,7 +2141,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:N10">
+  <conditionalFormatting sqref="C3:N10 C11:C20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2199,7 +2153,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:N20">
+  <conditionalFormatting sqref="D11:N20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>